<commit_message>
generating word files with data provided from excel
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -14,26 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>aaa</t>
-  </si>
-  <si>
-    <t>bbb</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t>bb</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,36 +352,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>